<commit_message>
Working on EIC notebook
</commit_message>
<xml_diff>
--- a/data/BA_Mapping.xlsx
+++ b/data/BA_Mapping.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burl878/Documents/Code/code_repos/ntp_heat_wave_loads/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CE3606-5904-4641-AB2A-D41313AA663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B027AC8-3D8F-5845-9010-5F06A1B52494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="680" windowWidth="16560" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="37940" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BA_to_Interconnection_Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="92">
   <si>
     <t>Interconnection</t>
   </si>
@@ -224,6 +237,78 @@
   </si>
   <si>
     <t>NEVP, SPPC</t>
+  </si>
+  <si>
+    <t>ISO-NE</t>
+  </si>
+  <si>
+    <t>NYISO</t>
+  </si>
+  <si>
+    <t>IESO, TE, NB, NS, CORNWALL, NF</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>BAs are in Canada and are thus not modeled by TELL</t>
+  </si>
+  <si>
+    <t>Name mismatch</t>
+  </si>
+  <si>
+    <t>BA is not modeled by TELL</t>
+  </si>
+  <si>
+    <t>CPLW</t>
+  </si>
+  <si>
+    <t>FTP, KEY, LWU, FMPP, RCU, TCEC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>FPL, OLEANDER</t>
+  </si>
+  <si>
+    <t>HE, DEI, SIGE, IPL, NIPS, METC, ITCT, WEC, MIUP, BREC, HMPL, LAGN, CWLD, SMEPA, EES, AMMO, AMIL, CWLP, SIPC, OMUA, CLEC, LAFA, LEPA, MJMEUC, SWPA, XEL, MP, SMMPA, GRE, OTP, ALTW, MEC, HAST, LES, MDU, BEPC-MISO, DPC, ALTE, WPS, MGE, UPPC</t>
+  </si>
+  <si>
+    <t>SOCO, GULF</t>
+  </si>
+  <si>
+    <t>EES-EMI, EES-EAI, AEPW, GRDA, OKGE, WFEC, SPS, OMPA, MIDW, SUNC, WERE, KCPL, KACY, EMDE, INDN, SPRM, NPPD, GRIS, OPPD, WAPA, BEPC-SPP</t>
+  </si>
+  <si>
+    <t>TECO, CALPINE</t>
+  </si>
+  <si>
+    <t>TVA, SMT</t>
+  </si>
+  <si>
+    <t>YAD</t>
+  </si>
+  <si>
+    <t>No match in GridView data</t>
+  </si>
+  <si>
+    <t>Generation only</t>
+  </si>
+  <si>
+    <t>ERCOT is not currently included in this study</t>
+  </si>
+  <si>
+    <t>APS, ATSI, AEP, OVEC, DAY, DEO&amp;K, DLCO, CE, PJM, PENELEC, ME, JCPL, PL, PECO, PSEG, BGE, PEPCO, AE, DP&amp;L, UGI, RECO, SMECO, EKPC, DVP</t>
+  </si>
+  <si>
+    <t>Assuming that APS = AP and that there was a typo in your mapping file</t>
+  </si>
+  <si>
+    <t>"CALPINE" doesn't show up in the GV data file</t>
   </si>
 </sst>
 </file>
@@ -721,7 +806,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -740,6 +825,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -800,9 +891,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -840,7 +931,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -946,7 +1037,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1088,7 +1179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1096,24 +1187,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="23.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1126,33 +1218,42 @@
       <c r="D1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1166,7 +1267,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1180,7 +1281,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1295,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1208,7 +1309,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1222,7 +1323,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1232,22 +1333,22 @@
       <c r="D9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1261,18 +1362,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1286,7 +1390,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1296,41 +1400,56 @@
       <c r="D14" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1344,29 +1463,35 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1380,7 +1505,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1390,33 +1515,42 @@
       <c r="D22" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1430,29 +1564,35 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1465,22 +1605,25 @@
       <c r="D28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1494,18 +1637,24 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1515,11 +1664,11 @@
       <c r="D32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1682,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1547,18 +1696,24 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +1727,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1586,7 +1741,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1600,29 +1755,35 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1636,40 +1797,49 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1683,40 +1853,52 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -1730,7 +1912,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +1926,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -1758,18 +1940,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1783,7 +1968,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -1797,7 +1982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1809,6 +1994,48 @@
       </c>
       <c r="D55" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>